<commit_message>
Tidy up tenant assessment
</commit_message>
<xml_diff>
--- a/Tenant Migration Assessment/TenantAssessment-Template.xlsx
+++ b/Tenant Migration Assessment/TenantAssessment-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\AdminSeanMc\Tenant Migration Assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F928ED0-445C-4A12-ADCC-4B8A7907560D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B8CE61-0C60-493D-86B7-0EB9E5EEA1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="High-Level" sheetId="25" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="125">
   <si>
     <t>Migrate</t>
   </si>
@@ -461,6 +461,24 @@
   </si>
   <si>
     <t>Additional Notes:</t>
+  </si>
+  <si>
+    <t>SharedChannels</t>
+  </si>
+  <si>
+    <t>SharedChannelSize</t>
+  </si>
+  <si>
+    <t>IncomingSharedChannels</t>
+  </si>
+  <si>
+    <t>Shared Channels</t>
+  </si>
+  <si>
+    <t>Incoming Shared Channels</t>
+  </si>
+  <si>
+    <t>Teams Shared Channel Data Size (GB)</t>
   </si>
 </sst>
 </file>
@@ -504,7 +522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
@@ -514,7 +532,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
@@ -541,6 +558,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,8 +578,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C81E16F-87D4-465B-9D71-E2F034FAE778}" name="Table1" displayName="Table1" ref="A2:B17" totalsRowShown="0">
-  <autoFilter ref="A2:B17" xr:uid="{8C81E16F-87D4-465B-9D71-E2F034FAE778}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C81E16F-87D4-465B-9D71-E2F034FAE778}" name="Table1" displayName="Table1" ref="A2:B20" totalsRowShown="0">
+  <autoFilter ref="A2:B20" xr:uid="{8C81E16F-87D4-465B-9D71-E2F034FAE778}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{9745AFED-DF63-40DF-91FD-BBFCFCDD2EEB}" name="Object"/>
     <tableColumn id="2" xr3:uid="{226A0CAD-C46B-4E71-972B-959E9A2A0C3D}" name="Value"/>
@@ -866,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18BF38E7-87BB-48B9-8B60-C799BBDAF6DD}">
-  <dimension ref="A2:B20"/>
+  <dimension ref="A2:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -988,42 +1007,69 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>112</v>
-      </c>
-      <c r="B14" cm="1">
-        <f t="array" ref="B14">ROUNDUP(SUM(((Teams!E2:E1048576)/1024)/1024)/1024,3)</f>
+        <v>122</v>
+      </c>
+      <c r="B14">
+        <f>SUM(Teams!E2:E1048576)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>113</v>
-      </c>
-      <c r="B15" cm="1">
-        <f t="array" ref="B15">ROUNDUP(SUM(((Teams!F2:F1048576)/1024)/1024)/1024,3)</f>
+        <v>123</v>
+      </c>
+      <c r="B15">
+        <f>SUM(Teams!I2:I1048576)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" cm="1">
+        <f t="array" ref="B16">ROUNDUP(SUM(((Teams!E2:E1048576)/1024)/1024)/1024,3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" cm="1">
+        <f t="array" ref="B17">ROUNDUP(SUM(((Teams!F2:F1048576)/1024)/1024)/1024,3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" cm="1">
+        <f t="array" ref="B18">ROUNDUP(SUM(((Teams!H2:H1048576)/1024)/1024)/1024,3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
         <v>115</v>
       </c>
-      <c r="B16">
+      <c r="B19">
         <f>COUNTA('User Accounts'!M:M)-1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
         <v>114</v>
       </c>
-      <c r="B17">
+      <c r="B20">
         <f>ROUNDUP(SUM('User Accounts'!L2:L1048576),3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1065,52 +1111,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="13" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1135,7 +1181,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="15"/>
+      <c r="A1" s="14"/>
     </row>
   </sheetData>
   <autoFilter ref="A1" xr:uid="{00000000-0009-0000-0000-000009000000}"/>
@@ -1167,72 +1213,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="16" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="I2" s="16"/>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="I3" s="16"/>
+      <c r="I3" s="15"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="I4" s="16"/>
+      <c r="I4" s="15"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="I5" s="16"/>
+      <c r="I5" s="15"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="I6" s="16"/>
+      <c r="I6" s="15"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="I7" s="16"/>
+      <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="I8" s="16"/>
+      <c r="I8" s="15"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="I9" s="16"/>
+      <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="I10" s="16"/>
+      <c r="I10" s="15"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="I11" s="16"/>
+      <c r="I11" s="15"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="I12" s="16"/>
+      <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="I13" s="16"/>
+      <c r="I13" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J13" xr:uid="{00000000-0009-0000-0000-00000A000000}"/>
@@ -1261,25 +1307,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1311,33 +1357,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="19" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="G2" s="19"/>
+      <c r="G2" s="18"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H2" xr:uid="{00000000-0009-0000-0000-00000C000000}"/>
@@ -1367,48 +1413,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="21" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="G2" s="21"/>
+      <c r="G2" s="20"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="G3" s="21"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="G4" s="21"/>
+      <c r="G4" s="20"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="G5" s="21"/>
+      <c r="G5" s="20"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="G6" s="21"/>
+      <c r="G6" s="20"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="G7" s="21"/>
+      <c r="G7" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H7" xr:uid="{00000000-0009-0000-0000-00000D000000}"/>
@@ -1438,33 +1484,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="G2" s="23"/>
+      <c r="G2" s="22"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H2" xr:uid="{00000000-0009-0000-0000-00000E000000}"/>
@@ -1493,25 +1539,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="24" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1545,63 +1591,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="26" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="I2" s="26"/>
+      <c r="I2" s="25"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="I4" s="26"/>
+      <c r="I4" s="25"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="I5" s="26"/>
+      <c r="I5" s="25"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="I7" s="26"/>
+      <c r="I7" s="25"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="I11" s="26"/>
+      <c r="I11" s="25"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="I13" s="26"/>
+      <c r="I13" s="25"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="I15" s="26"/>
+      <c r="I15" s="25"/>
     </row>
     <row r="17" spans="9:9">
-      <c r="I17" s="26"/>
+      <c r="I17" s="25"/>
     </row>
     <row r="20" spans="9:9">
-      <c r="I20" s="26"/>
+      <c r="I20" s="25"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J22" xr:uid="{00000000-0009-0000-0000-000010000000}"/>
@@ -1627,25 +1673,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E2" xr:uid="{00000000-0009-0000-0000-000011000000}"/>
@@ -1856,34 +1902,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="J1" s="29" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1912,19 +1958,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="30" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1953,22 +1999,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="31" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1993,7 +2039,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="33"/>
+      <c r="A1" s="32"/>
     </row>
   </sheetData>
   <autoFilter ref="A1" xr:uid="{00000000-0009-0000-0000-000015000000}"/>
@@ -2016,7 +2062,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="34"/>
+      <c r="A1" s="33"/>
     </row>
   </sheetData>
   <autoFilter ref="A1" xr:uid="{00000000-0009-0000-0000-000016000000}"/>
@@ -2049,37 +2095,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="K1" s="34" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2425,11 +2471,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD12"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2438,7 +2484,7 @@
     <col min="2" max="2" width="29.5703125" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="60.28515625" customWidth="1"/>
     <col min="8" max="8" width="69.5703125" customWidth="1"/>
@@ -2451,94 +2497,103 @@
     <col min="15" max="15" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:18" s="36" customFormat="1">
+      <c r="A1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="K1" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="L1" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="M1" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="N1" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="O1" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="P1" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="Q1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="R1" s="35" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:18">
       <c r="H2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:18">
       <c r="H3" s="8"/>
       <c r="N3" s="8"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:18">
       <c r="H4" s="8"/>
       <c r="N4" s="8"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:18">
       <c r="H5" s="8"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:18">
       <c r="H6" s="8"/>
       <c r="N6" s="8"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:18">
       <c r="H7" s="8"/>
       <c r="N7" s="8"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:18">
       <c r="H8" s="8"/>
       <c r="N8" s="8"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:18">
       <c r="H9" s="8"/>
       <c r="N9" s="8"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:18">
       <c r="H10" s="8"/>
       <c r="N10" s="8"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:18">
       <c r="H11" s="8"/>
       <c r="N11" s="8"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:18">
       <c r="H12" s="8"/>
       <c r="N12" s="8"/>
     </row>
@@ -2574,45 +2629,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="H2" s="10"/>
+      <c r="H2" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L2" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
@@ -2638,16 +2693,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2674,9 +2729,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="A1" s="12"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated tenant assessment template sheet
</commit_message>
<xml_diff>
--- a/Tenant Migration Assessment/TenantAssessment-Template.xlsx
+++ b/Tenant Migration Assessment/TenantAssessment-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\AdminSeanMc\Tenant Migration Assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAB9323-7A29-497D-8550-F6C254964BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BED394-1DDD-45B7-808E-A9E12FCC34F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="High-Level" sheetId="25" r:id="rId1"/>
@@ -836,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18BF38E7-87BB-48B9-8B60-C799BBDAF6DD}">
   <dimension ref="A2:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -977,7 +977,7 @@
         <v>101</v>
       </c>
       <c r="B16" cm="1">
-        <f t="array" ref="B16">ROUNDUP(SUM(((Teams!E2:E1048576)/1024)/1024)/1024,3)</f>
+        <f t="array" ref="B16">ROUNDUP(SUM(((Teams!F2:F1048576)/1024)/1024)/1024,3)</f>
         <v>0</v>
       </c>
     </row>
@@ -986,7 +986,7 @@
         <v>102</v>
       </c>
       <c r="B17" cm="1">
-        <f t="array" ref="B17">ROUNDUP(SUM(((Teams!F2:F1048576)/1024)/1024)/1024,3)</f>
+        <f t="array" ref="B17">ROUNDUP(SUM(((Teams!G2:G1048576)/1024)/1024)/1024,3)</f>
         <v>0</v>
       </c>
     </row>
@@ -1216,7 +1216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
@@ -2118,9 +2118,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>